<commit_message>
Updated Status And Requirements
</commit_message>
<xml_diff>
--- a/ProjectDocuments/01_Planning/11_Gantt_Project_Plan.xlsx
+++ b/ProjectDocuments/01_Planning/11_Gantt_Project_Plan.xlsx
@@ -1,32 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReqM_project\ProjectDocuments\01_Planning\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510"/>
   </bookViews>
   <sheets>
-    <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
+    <sheet name="Cover" sheetId="2" r:id="rId1"/>
+    <sheet name="Requirements" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Actual">(PeriodInActual*('Project Planner'!$E1&gt;0))*PeriodInPlan</definedName>
-    <definedName name="ActualBeyond">PeriodInActual*('Project Planner'!$E1&gt;0)</definedName>
+    <definedName name="Actual">(PeriodInActual*(Requirements!$E1&gt;0))*PeriodInPlan</definedName>
+    <definedName name="ActualBeyond">PeriodInActual*(Requirements!$E1&gt;0)</definedName>
     <definedName name="PercentComplete">PercentCompleteBeyond*PeriodInPlan</definedName>
-    <definedName name="PercentCompleteBeyond">('Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$E1,'Project Planner'!$E1+'Project Planner'!$F1)*('Project Planner'!$E1&gt;0))*(('Project Planner'!A$4&lt;(INT('Project Planner'!$E1+'Project Planner'!$F1*'Project Planner'!$G1)))+('Project Planner'!A$4='Project Planner'!$E1))*('Project Planner'!$G1&gt;0)</definedName>
-    <definedName name="period_selected">'Project Planner'!$I$2</definedName>
-    <definedName name="PeriodInActual">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$E1,'Project Planner'!$E1+'Project Planner'!$F1-1)</definedName>
-    <definedName name="PeriodInPlan">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$C1,'Project Planner'!$C1+'Project Planner'!$D1-1)</definedName>
-    <definedName name="Plan">PeriodInPlan*('Project Planner'!$C1&gt;0)</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Planner'!$3:$4</definedName>
-    <definedName name="TitleRegion..BO60">'Project Planner'!$B$3:$B$4</definedName>
+    <definedName name="PercentCompleteBeyond">(Requirements!A$4=MEDIAN(Requirements!A$4,Requirements!$E1,Requirements!$E1+Requirements!$F1)*(Requirements!$E1&gt;0))*((Requirements!A$4&lt;(INT(Requirements!$E1+Requirements!$F1*Requirements!$G1)))+(Requirements!A$4=Requirements!$E1))*(Requirements!$G1&gt;0)</definedName>
+    <definedName name="period_selected">Requirements!$I$2</definedName>
+    <definedName name="PeriodInActual">Requirements!A$4=MEDIAN(Requirements!A$4,Requirements!$E1,Requirements!$E1+Requirements!$F1-1)</definedName>
+    <definedName name="PeriodInPlan">Requirements!A$4=MEDIAN(Requirements!A$4,Requirements!$C1,Requirements!$C1+Requirements!$D1-1)</definedName>
+    <definedName name="Plan">PeriodInPlan*(Requirements!$C1&gt;0)</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">Requirements!$3:$4</definedName>
+    <definedName name="TitleRegion..BO60">Requirements!$B$3:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="116">
   <si>
     <t>Project Planner</t>
   </si>
@@ -391,12 +387,81 @@
   <si>
     <t>Rares</t>
   </si>
+  <si>
+    <t>Summary:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author </t>
+  </si>
+  <si>
+    <t>Function/Department</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Signature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approved by </t>
+  </si>
+  <si>
+    <t>Madalina Fantana</t>
+  </si>
+  <si>
+    <t>Gantt Chart</t>
+  </si>
+  <si>
+    <t>R.A.D.U. - Requirements And Design Utility</t>
+  </si>
+  <si>
+    <t>Project:</t>
+  </si>
+  <si>
+    <t>Document Description:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gantt Chart is bar chart of schedule information where </t>
+  </si>
+  <si>
+    <t xml:space="preserve">activities are listed on the vertical axis, dates are shown </t>
+  </si>
+  <si>
+    <t xml:space="preserve">on the horizontal axis, and activity durations are shown </t>
+  </si>
+  <si>
+    <t>as horizontal bars placed according to start and finish dates.</t>
+  </si>
+  <si>
+    <t>Req076</t>
+  </si>
+  <si>
+    <t>Req077</t>
+  </si>
+  <si>
+    <t>Req078</t>
+  </si>
+  <si>
+    <t>Req079</t>
+  </si>
+  <si>
+    <t>Req080</t>
+  </si>
+  <si>
+    <t>Req081</t>
+  </si>
+  <si>
+    <t>Req082</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -496,8 +561,58 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -539,8 +654,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -625,6 +746,138 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -683,7 +936,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -795,6 +1048,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="% complete" xfId="16"/>
@@ -817,7 +1120,7 @@
     <cellStyle name="Project Headers" xfId="4"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="245">
     <dxf>
       <fill>
         <patternFill>
@@ -1386,6 +1689,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1397,19 +1728,75 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="7"/>
-        </top>
-        <vertical/>
-        <horizontal/>
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1523,6 +1910,2620 @@
         <bottom style="thin">
           <color theme="0"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="7"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -1536,6 +4537,173 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9365</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>59001</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524215" y="7831401"/>
+          <a:ext cx="962185" cy="417250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="600" b="1" cap="small">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>NTT Data Romania S.A.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="600">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="600" b="1" cap="small">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>19-21, Constanta Street,</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="600">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="600" b="1" cap="small">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>400158 Cluj Napoca</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="300">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1027" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4086225" y="19050"/>
+          <a:ext cx="1752600" cy="447675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1764,18 +4932,446 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.875" style="40" customWidth="1"/>
+    <col min="2" max="2" width="17.125" style="40" customWidth="1"/>
+    <col min="3" max="3" width="25.875" style="40" customWidth="1"/>
+    <col min="4" max="4" width="11.375" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.875" style="40" customWidth="1"/>
+    <col min="6" max="6" width="4.875" style="40" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="40"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="39"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="41"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="43"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="43"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75">
+      <c r="A5" s="44"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="46"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75">
+      <c r="A6" s="41"/>
+      <c r="B6" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="42"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="48"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="41"/>
+      <c r="B7" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="43"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="41"/>
+      <c r="B8" s="61" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="43"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="41"/>
+      <c r="B9" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="43"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="41"/>
+      <c r="B10" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="43"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="41"/>
+      <c r="B11" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="43"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="41"/>
+      <c r="B12" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="43"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="41"/>
+      <c r="B13" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="41"/>
+      <c r="B14" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="43"/>
+    </row>
+    <row r="16" spans="1:7" ht="16.5" thickBot="1">
+      <c r="A16" s="41"/>
+      <c r="B16" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="43"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A17" s="41"/>
+      <c r="B17" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="53"/>
+      <c r="D17" s="54">
+        <v>43656</v>
+      </c>
+      <c r="E17" s="53"/>
+      <c r="F17" s="43"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A18" s="41"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="43"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A19" s="41"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="43"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A20" s="41"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="43"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="41"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="43"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="41"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="43"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="41"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="43"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="41"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="43"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="43"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="43"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="41"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="43"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="41"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="43"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="41"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="43"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="41"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="43"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="41"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="43"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="41"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="43"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="41"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="43"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="41"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="43"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A35" s="41"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="43"/>
+    </row>
+    <row r="36" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A36" s="41"/>
+      <c r="B36" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="43"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A37" s="41"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="43"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A38" s="41"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="43"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A39" s="41"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="43"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A40" s="41"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="43"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="41"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="43"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="41"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="43"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="41"/>
+      <c r="B43" s="42"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="43"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="41"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="43"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="41"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="43"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="55"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="57"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:E5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BP79"/>
+  <dimension ref="B1:BP90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AB58" sqref="AB58"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="2" customWidth="1"/>
@@ -1784,7 +5380,7 @@
     <col min="9" max="28" width="2.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:68" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="2:68" ht="60" customHeight="1" thickBot="1">
       <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1795,7 +5391,7 @@
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
     </row>
-    <row r="2" spans="2:68" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:68" ht="21" customHeight="1" thickTop="1" thickBot="1">
       <c r="B2" s="23" t="s">
         <v>89</v>
       </c>
@@ -1854,7 +5450,7 @@
       <c r="AP2" s="22"/>
       <c r="AQ2" s="22"/>
     </row>
-    <row r="3" spans="2:68" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:68" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
       <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
@@ -1899,7 +5495,7 @@
       <c r="AA3" s="10"/>
       <c r="AB3" s="10"/>
     </row>
-    <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:68" ht="15.75" customHeight="1">
       <c r="B4" s="25"/>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -2088,7 +5684,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:68" ht="30" customHeight="1">
       <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
@@ -2111,7 +5707,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:68" ht="30" customHeight="1">
       <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
@@ -2134,8 +5730,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="6" t="s">
+    <row r="7" spans="2:68" ht="30" customHeight="1">
+      <c r="B7" s="62" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="7">
@@ -2155,7 +5751,7 @@
       </c>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:68" ht="30" customHeight="1">
       <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
@@ -2178,7 +5774,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:68" ht="30" customHeight="1">
       <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
@@ -2201,7 +5797,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:68" ht="30" customHeight="1">
       <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
@@ -2224,7 +5820,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:68" ht="30" customHeight="1">
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
@@ -2247,7 +5843,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:68" ht="30" customHeight="1">
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
@@ -2270,7 +5866,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:68" ht="30" customHeight="1">
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
@@ -2293,7 +5889,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:68" ht="30" customHeight="1">
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
@@ -2316,7 +5912,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:68" ht="30" customHeight="1">
       <c r="B15" s="6" t="s">
         <v>24</v>
       </c>
@@ -2339,7 +5935,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:68" ht="30" customHeight="1">
       <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
@@ -2362,7 +5958,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="30" customHeight="1">
       <c r="B17" s="6" t="s">
         <v>26</v>
       </c>
@@ -2385,7 +5981,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" ht="30" customHeight="1">
       <c r="B18" s="6" t="s">
         <v>27</v>
       </c>
@@ -2408,7 +6004,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" ht="30" customHeight="1">
       <c r="B19" s="6" t="s">
         <v>28</v>
       </c>
@@ -2431,7 +6027,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="30" customHeight="1">
       <c r="B20" s="6" t="s">
         <v>29</v>
       </c>
@@ -2454,7 +6050,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" ht="30" customHeight="1">
       <c r="B21" s="6" t="s">
         <v>30</v>
       </c>
@@ -2477,7 +6073,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="30" customHeight="1">
       <c r="B22" s="6" t="s">
         <v>31</v>
       </c>
@@ -2500,7 +6096,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="30" customHeight="1">
       <c r="B23" s="6" t="s">
         <v>32</v>
       </c>
@@ -2523,7 +6119,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" ht="30" customHeight="1">
       <c r="B24" s="6" t="s">
         <v>33</v>
       </c>
@@ -2546,7 +6142,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="30" customHeight="1">
       <c r="B25" s="6" t="s">
         <v>34</v>
       </c>
@@ -2569,7 +6165,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" ht="30" customHeight="1">
       <c r="B26" s="6" t="s">
         <v>35</v>
       </c>
@@ -2592,7 +6188,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" ht="30" customHeight="1">
       <c r="B27" s="6" t="s">
         <v>36</v>
       </c>
@@ -2615,7 +6211,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" ht="30" customHeight="1">
       <c r="B28" s="6" t="s">
         <v>37</v>
       </c>
@@ -2638,7 +6234,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" ht="30" customHeight="1">
       <c r="B29" s="6" t="s">
         <v>38</v>
       </c>
@@ -2661,7 +6257,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" ht="30" customHeight="1">
       <c r="B30" s="6" t="s">
         <v>39</v>
       </c>
@@ -2684,7 +6280,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" ht="30" customHeight="1">
       <c r="B31" s="6" t="s">
         <v>40</v>
       </c>
@@ -2707,7 +6303,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" ht="30" customHeight="1">
       <c r="B32" s="6" t="s">
         <v>41</v>
       </c>
@@ -2730,7 +6326,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" ht="30" customHeight="1">
       <c r="B33" s="6" t="s">
         <v>42</v>
       </c>
@@ -2753,7 +6349,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:8" ht="30" customHeight="1">
       <c r="B34" s="6" t="s">
         <v>43</v>
       </c>
@@ -2776,7 +6372,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" ht="30" customHeight="1">
       <c r="B35" s="6" t="s">
         <v>44</v>
       </c>
@@ -2799,7 +6395,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" ht="30" customHeight="1">
       <c r="B36" s="6" t="s">
         <v>45</v>
       </c>
@@ -2822,7 +6418,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" ht="30" customHeight="1">
       <c r="B37" s="6" t="s">
         <v>46</v>
       </c>
@@ -2845,7 +6441,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" ht="30" customHeight="1">
       <c r="B38" s="6" t="s">
         <v>47</v>
       </c>
@@ -2868,7 +6464,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" ht="30" customHeight="1">
       <c r="B39" s="6" t="s">
         <v>48</v>
       </c>
@@ -2891,7 +6487,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:8" ht="30" customHeight="1">
       <c r="B40" s="6" t="s">
         <v>49</v>
       </c>
@@ -2914,7 +6510,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" ht="30" customHeight="1">
       <c r="B41" s="6" t="s">
         <v>50</v>
       </c>
@@ -2937,7 +6533,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" ht="30" customHeight="1">
       <c r="B42" s="6" t="s">
         <v>51</v>
       </c>
@@ -2960,7 +6556,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:8" ht="30" customHeight="1">
       <c r="B43" s="6" t="s">
         <v>52</v>
       </c>
@@ -2983,8 +6579,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="6" t="s">
+    <row r="44" spans="2:8" ht="30" customHeight="1">
+      <c r="B44" s="62" t="s">
         <v>53</v>
       </c>
       <c r="C44" s="7">
@@ -3004,7 +6600,7 @@
       </c>
       <c r="H44" s="8"/>
     </row>
-    <row r="45" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" ht="30" customHeight="1">
       <c r="B45" s="6" t="s">
         <v>54</v>
       </c>
@@ -3025,7 +6621,7 @@
       </c>
       <c r="H45" s="8"/>
     </row>
-    <row r="46" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:8" ht="30" customHeight="1">
       <c r="B46" s="6" t="s">
         <v>55</v>
       </c>
@@ -3046,7 +6642,7 @@
       </c>
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:8" ht="30" customHeight="1">
       <c r="B47" s="6" t="s">
         <v>56</v>
       </c>
@@ -3067,7 +6663,7 @@
       </c>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:8" ht="30" customHeight="1">
       <c r="B48" s="6" t="s">
         <v>57</v>
       </c>
@@ -3088,7 +6684,7 @@
       </c>
       <c r="H48" s="8"/>
     </row>
-    <row r="49" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:8" ht="30" customHeight="1">
       <c r="B49" s="6" t="s">
         <v>58</v>
       </c>
@@ -3109,7 +6705,7 @@
       </c>
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:8" ht="30" customHeight="1">
       <c r="B50" s="6" t="s">
         <v>59</v>
       </c>
@@ -3130,7 +6726,7 @@
       </c>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:8" ht="30" customHeight="1">
       <c r="B51" s="6" t="s">
         <v>60</v>
       </c>
@@ -3153,7 +6749,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:8" ht="30" customHeight="1">
       <c r="B52" s="6" t="s">
         <v>61</v>
       </c>
@@ -3173,7 +6769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:8" ht="30" customHeight="1">
       <c r="B53" s="6" t="s">
         <v>62</v>
       </c>
@@ -3194,7 +6790,7 @@
       </c>
       <c r="H53" s="8"/>
     </row>
-    <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:8" ht="30" customHeight="1">
       <c r="B54" s="6" t="s">
         <v>63</v>
       </c>
@@ -3215,7 +6811,7 @@
       </c>
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:8" ht="30" customHeight="1">
       <c r="B55" s="6" t="s">
         <v>64</v>
       </c>
@@ -3236,7 +6832,7 @@
       </c>
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:8" ht="30" customHeight="1">
       <c r="B56" s="6" t="s">
         <v>65</v>
       </c>
@@ -3257,8 +6853,8 @@
       </c>
       <c r="H56" s="8"/>
     </row>
-    <row r="57" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="6" t="s">
+    <row r="57" spans="2:8" ht="30" customHeight="1">
+      <c r="B57" s="62" t="s">
         <v>66</v>
       </c>
       <c r="C57" s="7">
@@ -3280,7 +6876,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:8" ht="30" customHeight="1">
       <c r="B58" s="6" t="s">
         <v>67</v>
       </c>
@@ -3303,7 +6899,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:8" ht="30" customHeight="1">
       <c r="B59" s="6" t="s">
         <v>68</v>
       </c>
@@ -3320,14 +6916,14 @@
         <v>2</v>
       </c>
       <c r="G59" s="8">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="H59" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="6" t="s">
+    <row r="60" spans="2:8" ht="30" customHeight="1">
+      <c r="B60" s="62" t="s">
         <v>69</v>
       </c>
       <c r="C60" s="7">
@@ -3349,7 +6945,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:8" ht="30" customHeight="1">
       <c r="B61" s="6" t="s">
         <v>70</v>
       </c>
@@ -3368,11 +6964,9 @@
       <c r="G61" s="8">
         <v>1</v>
       </c>
-      <c r="H61" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H61" s="8"/>
+    </row>
+    <row r="62" spans="2:8" ht="30" customHeight="1">
       <c r="B62" s="6" t="s">
         <v>71</v>
       </c>
@@ -3393,7 +6987,7 @@
       </c>
       <c r="H62" s="8"/>
     </row>
-    <row r="63" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:8" ht="30" customHeight="1">
       <c r="B63" s="6" t="s">
         <v>72</v>
       </c>
@@ -3414,7 +7008,7 @@
       </c>
       <c r="H63" s="8"/>
     </row>
-    <row r="64" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:8" ht="30" customHeight="1">
       <c r="B64" s="6" t="s">
         <v>73</v>
       </c>
@@ -3435,7 +7029,7 @@
       </c>
       <c r="H64" s="8"/>
     </row>
-    <row r="65" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:8" ht="30" customHeight="1">
       <c r="B65" s="6" t="s">
         <v>74</v>
       </c>
@@ -3456,7 +7050,7 @@
       </c>
       <c r="H65" s="8"/>
     </row>
-    <row r="66" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:8" ht="30" customHeight="1">
       <c r="B66" s="6" t="s">
         <v>75</v>
       </c>
@@ -3477,7 +7071,7 @@
       </c>
       <c r="H66" s="8"/>
     </row>
-    <row r="67" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:8" ht="30" customHeight="1">
       <c r="B67" s="6" t="s">
         <v>76</v>
       </c>
@@ -3498,7 +7092,7 @@
       </c>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:8" ht="30" customHeight="1">
       <c r="B68" s="6" t="s">
         <v>77</v>
       </c>
@@ -3519,7 +7113,7 @@
       </c>
       <c r="H68" s="8"/>
     </row>
-    <row r="69" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:8" ht="30" customHeight="1">
       <c r="B69" s="6" t="s">
         <v>78</v>
       </c>
@@ -3540,7 +7134,7 @@
       </c>
       <c r="H69" s="8"/>
     </row>
-    <row r="70" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:8" ht="30" customHeight="1">
       <c r="B70" s="6" t="s">
         <v>79</v>
       </c>
@@ -3561,7 +7155,7 @@
       </c>
       <c r="H70" s="8"/>
     </row>
-    <row r="71" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:8" ht="30" customHeight="1">
       <c r="B71" s="6" t="s">
         <v>80</v>
       </c>
@@ -3582,8 +7176,8 @@
       </c>
       <c r="H71" s="8"/>
     </row>
-    <row r="72" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="6" t="s">
+    <row r="72" spans="2:8" ht="30" customHeight="1">
+      <c r="B72" s="62" t="s">
         <v>81</v>
       </c>
       <c r="C72" s="7">
@@ -3605,7 +7199,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="73" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:8" ht="30" customHeight="1">
       <c r="B73" s="6" t="s">
         <v>82</v>
       </c>
@@ -3628,7 +7222,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="74" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:8" ht="30" customHeight="1">
       <c r="B74" s="6" t="s">
         <v>83</v>
       </c>
@@ -3649,7 +7243,7 @@
       </c>
       <c r="H74" s="8"/>
     </row>
-    <row r="75" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:8" ht="30" customHeight="1">
       <c r="B75" s="6" t="s">
         <v>84</v>
       </c>
@@ -3670,7 +7264,7 @@
       </c>
       <c r="H75" s="8"/>
     </row>
-    <row r="76" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:8" ht="30" customHeight="1">
       <c r="B76" s="6" t="s">
         <v>85</v>
       </c>
@@ -3691,7 +7285,7 @@
       </c>
       <c r="H76" s="8"/>
     </row>
-    <row r="77" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:8" ht="30" customHeight="1">
       <c r="B77" s="6" t="s">
         <v>86</v>
       </c>
@@ -3712,7 +7306,7 @@
       </c>
       <c r="H77" s="8"/>
     </row>
-    <row r="78" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:8" ht="30" customHeight="1">
       <c r="B78" s="6" t="s">
         <v>87</v>
       </c>
@@ -3733,7 +7327,7 @@
       </c>
       <c r="H78" s="8"/>
     </row>
-    <row r="79" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:8" ht="30" customHeight="1">
       <c r="B79" s="6" t="s">
         <v>88</v>
       </c>
@@ -3753,6 +7347,207 @@
         <v>0</v>
       </c>
       <c r="H79" s="8"/>
+    </row>
+    <row r="80" spans="2:8" ht="30" customHeight="1">
+      <c r="B80" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="C80" s="7">
+        <v>2</v>
+      </c>
+      <c r="D80" s="7">
+        <v>0</v>
+      </c>
+      <c r="E80" s="7">
+        <v>2</v>
+      </c>
+      <c r="F80" s="7">
+        <v>0</v>
+      </c>
+      <c r="G80" s="8">
+        <v>1</v>
+      </c>
+      <c r="H80" s="8"/>
+    </row>
+    <row r="81" spans="2:28" ht="30" customHeight="1">
+      <c r="B81" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="C81" s="7">
+        <v>2</v>
+      </c>
+      <c r="D81" s="7">
+        <v>0</v>
+      </c>
+      <c r="E81" s="7">
+        <v>2</v>
+      </c>
+      <c r="F81" s="7">
+        <v>0</v>
+      </c>
+      <c r="G81" s="8">
+        <v>1</v>
+      </c>
+      <c r="H81" s="8"/>
+    </row>
+    <row r="82" spans="2:28" ht="30" customHeight="1">
+      <c r="B82" s="62" t="s">
+        <v>111</v>
+      </c>
+      <c r="C82" s="7">
+        <v>2</v>
+      </c>
+      <c r="D82" s="7">
+        <v>0</v>
+      </c>
+      <c r="E82" s="7">
+        <v>2</v>
+      </c>
+      <c r="F82" s="7">
+        <v>0</v>
+      </c>
+      <c r="G82" s="8">
+        <v>1</v>
+      </c>
+      <c r="H82" s="8"/>
+    </row>
+    <row r="83" spans="2:28" ht="30" customHeight="1">
+      <c r="B83" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="C83" s="7">
+        <v>2</v>
+      </c>
+      <c r="D83" s="7">
+        <v>0</v>
+      </c>
+      <c r="E83" s="7">
+        <v>2</v>
+      </c>
+      <c r="F83" s="7">
+        <v>0</v>
+      </c>
+      <c r="G83" s="8">
+        <v>1</v>
+      </c>
+      <c r="H83" s="8"/>
+    </row>
+    <row r="84" spans="2:28" ht="30" customHeight="1">
+      <c r="B84" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="C84" s="7">
+        <v>2</v>
+      </c>
+      <c r="D84" s="7">
+        <v>0</v>
+      </c>
+      <c r="E84" s="7">
+        <v>2</v>
+      </c>
+      <c r="F84" s="7">
+        <v>0</v>
+      </c>
+      <c r="G84" s="8">
+        <v>0</v>
+      </c>
+      <c r="H84" s="8"/>
+    </row>
+    <row r="85" spans="2:28" ht="30" customHeight="1">
+      <c r="B85" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="C85" s="7">
+        <v>2</v>
+      </c>
+      <c r="D85" s="7">
+        <v>0</v>
+      </c>
+      <c r="E85" s="7">
+        <v>2</v>
+      </c>
+      <c r="F85" s="7">
+        <v>0</v>
+      </c>
+      <c r="G85" s="8">
+        <v>0</v>
+      </c>
+      <c r="H85" s="8"/>
+    </row>
+    <row r="86" spans="2:28" ht="30" customHeight="1">
+      <c r="B86" s="62" t="s">
+        <v>115</v>
+      </c>
+      <c r="C86" s="7">
+        <v>2</v>
+      </c>
+      <c r="D86" s="7">
+        <v>0</v>
+      </c>
+      <c r="E86" s="7">
+        <v>2</v>
+      </c>
+      <c r="F86" s="7">
+        <v>0</v>
+      </c>
+      <c r="G86" s="8">
+        <v>1</v>
+      </c>
+      <c r="H86" s="8"/>
+    </row>
+    <row r="87" spans="2:28" ht="30" customHeight="1">
+      <c r="B87" s="63"/>
+      <c r="C87" s="63"/>
+      <c r="D87" s="63"/>
+      <c r="E87" s="63"/>
+      <c r="F87" s="63"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="R87"/>
+      <c r="S87"/>
+      <c r="T87"/>
+      <c r="U87"/>
+      <c r="V87"/>
+      <c r="W87"/>
+      <c r="X87"/>
+      <c r="Y87"/>
+      <c r="Z87"/>
+      <c r="AA87"/>
+      <c r="AB87"/>
+    </row>
+    <row r="88" spans="2:28" ht="30" customHeight="1">
+      <c r="B88" s="63"/>
+      <c r="C88" s="63"/>
+      <c r="D88" s="63"/>
+      <c r="E88" s="63"/>
+      <c r="F88" s="63"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="R88"/>
+      <c r="S88"/>
+      <c r="T88"/>
+      <c r="U88"/>
+      <c r="V88"/>
+      <c r="W88"/>
+      <c r="X88"/>
+      <c r="Y88"/>
+      <c r="Z88"/>
+      <c r="AA88"/>
+      <c r="AB88"/>
+    </row>
+    <row r="89" spans="2:28" ht="30" customHeight="1">
+      <c r="B89" s="64"/>
+      <c r="C89" s="63"/>
+      <c r="D89" s="63"/>
+      <c r="E89" s="63"/>
+      <c r="F89" s="63"/>
+    </row>
+    <row r="90" spans="2:28" ht="30" customHeight="1">
+      <c r="B90" s="64"/>
+      <c r="C90" s="63"/>
+      <c r="D90" s="63"/>
+      <c r="E90" s="63"/>
+      <c r="F90" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -3770,169 +7565,195 @@
     <mergeCell ref="AB2:AH2"/>
     <mergeCell ref="H3:H4"/>
   </mergeCells>
-  <conditionalFormatting sqref="I32:BP32 I34:BP57 I79:BP79">
-    <cfRule type="expression" dxfId="49" priority="41">
+  <conditionalFormatting sqref="I32:BP32 I34:BP57 I79:BP85">
+    <cfRule type="expression" dxfId="209" priority="130">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="43">
+    <cfRule type="expression" dxfId="208" priority="132">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="44">
+    <cfRule type="expression" dxfId="207" priority="133">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="45">
+    <cfRule type="expression" dxfId="206" priority="134">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="46">
+    <cfRule type="expression" dxfId="205" priority="135">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="47">
+    <cfRule type="expression" dxfId="204" priority="136">
       <formula>I$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="51">
+    <cfRule type="expression" dxfId="203" priority="140">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="52">
+    <cfRule type="expression" dxfId="202" priority="141">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B80:BP80">
-    <cfRule type="expression" dxfId="41" priority="42">
+  <conditionalFormatting sqref="O80:BP80">
+    <cfRule type="expression" dxfId="201" priority="131">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:BP4">
-    <cfRule type="expression" dxfId="40" priority="48">
+    <cfRule type="expression" dxfId="200" priority="137">
       <formula>I$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:BP33">
-    <cfRule type="expression" dxfId="39" priority="33">
+    <cfRule type="expression" dxfId="199" priority="122">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="34">
+    <cfRule type="expression" dxfId="198" priority="123">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="35">
+    <cfRule type="expression" dxfId="197" priority="124">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="36">
+    <cfRule type="expression" dxfId="196" priority="125">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="37">
+    <cfRule type="expression" dxfId="195" priority="126">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="38">
+    <cfRule type="expression" dxfId="194" priority="127">
       <formula>I$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="39">
+    <cfRule type="expression" dxfId="193" priority="128">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="40">
+    <cfRule type="expression" dxfId="192" priority="129">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:BP5 I7:BP31">
-    <cfRule type="expression" dxfId="31" priority="25">
+    <cfRule type="expression" dxfId="191" priority="114">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="26">
+    <cfRule type="expression" dxfId="190" priority="115">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="27">
+    <cfRule type="expression" dxfId="189" priority="116">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="28">
+    <cfRule type="expression" dxfId="188" priority="117">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="29">
+    <cfRule type="expression" dxfId="187" priority="118">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="30">
+    <cfRule type="expression" dxfId="186" priority="119">
       <formula>I$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="31">
+    <cfRule type="expression" dxfId="185" priority="120">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="32">
+    <cfRule type="expression" dxfId="184" priority="121">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BP6">
-    <cfRule type="expression" dxfId="23" priority="17">
+    <cfRule type="expression" dxfId="183" priority="106">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="18">
+    <cfRule type="expression" dxfId="182" priority="107">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="19">
+    <cfRule type="expression" dxfId="181" priority="108">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="20">
+    <cfRule type="expression" dxfId="180" priority="109">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="21">
+    <cfRule type="expression" dxfId="179" priority="110">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="22">
+    <cfRule type="expression" dxfId="178" priority="111">
       <formula>I$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="23">
+    <cfRule type="expression" dxfId="177" priority="112">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="24">
+    <cfRule type="expression" dxfId="176" priority="113">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I58:BP58 I60:BP78">
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="175" priority="98">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="10">
+    <cfRule type="expression" dxfId="174" priority="99">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="173" priority="100">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="12">
+    <cfRule type="expression" dxfId="172" priority="101">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="171" priority="102">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14">
+    <cfRule type="expression" dxfId="170" priority="103">
       <formula>I$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="15">
+    <cfRule type="expression" dxfId="169" priority="104">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="16">
+    <cfRule type="expression" dxfId="168" priority="105">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I59:BP59">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="167" priority="90">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="166" priority="91">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="165" priority="92">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="164" priority="93">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="163" priority="94">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="162" priority="95">
       <formula>I$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="161" priority="96">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="160" priority="97">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I86:BP86">
+    <cfRule type="expression" dxfId="15" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="6">
+      <formula>I$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>